<commit_message>
fix(unit test): correct expected outcomes of crosstab_percent
</commit_message>
<xml_diff>
--- a/tests/test-data/crosstab-mean-inputs.xlsx
+++ b/tests/test-data/crosstab-mean-inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\dev\dataduck\tests\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED74713-4AF7-4EE9-A281-6F9AC43F53A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E581888E-E184-416E-B7E0-9E9B205353AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="240" windowWidth="25665" windowHeight="20505" xr2:uid="{92061F1E-9ABC-447A-B522-1CC605CAA3B1}"/>
   </bookViews>
@@ -1032,7 +1032,7 @@
   <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,8 +1652,8 @@
         <v>9.6168899101746627E-2</v>
       </c>
       <c r="R19">
-        <f>(4/80)*SQRT(SUM(N19:Q19))</f>
-        <v>0.14438684669678603</v>
+        <f>SQRT((4/80)*SUM(N19:Q19))</f>
+        <v>0.64571760854170901</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -1723,8 +1723,8 @@
         <v>0.58816855932036494</v>
       </c>
       <c r="R20">
-        <f t="shared" ref="R20:R23" si="4">(4/80)*SQRT(SUM(N20:Q20))</f>
-        <v>0.30194954244584887</v>
+        <f t="shared" ref="R20:R23" si="4">SQRT((4/80)*SUM(N20:Q20))</f>
+        <v>1.3503594053677523</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -1795,7 +1795,7 @@
       </c>
       <c r="R21">
         <f t="shared" si="4"/>
-        <v>0.27783846618218028</v>
+        <v>1.2425313942952629</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="R22">
         <f t="shared" si="4"/>
-        <v>0.32696163116889132</v>
+        <v>1.46221686665571</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -1937,7 +1937,7 @@
       </c>
       <c r="R23">
         <f t="shared" si="4"/>
-        <v>0.32696163116889149</v>
+        <v>1.4622168666557107</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -2063,7 +2063,7 @@
         <v>0</v>
       </c>
       <c r="R27">
-        <f>(4/80)*SQRT(SUM(N27:Q27))</f>
+        <f>SQRT((4/80)*SUM(N27:Q27))</f>
         <v>0</v>
       </c>
     </row>
@@ -2129,8 +2129,8 @@
         <v>0.35222382769272953</v>
       </c>
       <c r="R28">
-        <f t="shared" ref="R28:R31" si="12">(4/80)*SQRT(SUM(N28:Q28))</f>
-        <v>0.6451716111424366</v>
+        <f t="shared" ref="R28:R31" si="12">SQRT((4/80)*SUM(N28:Q28))</f>
+        <v>2.8852951593350982</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -2262,7 +2262,7 @@
       </c>
       <c r="R30">
         <f t="shared" si="12"/>
-        <v>0.64517161114243637</v>
+        <v>2.8852951593350968</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
test(crosstab_count): adjust unit test to match new output format
Unit test is currently failing.
</commit_message>
<xml_diff>
--- a/tests/test-data/crosstab-mean-inputs.xlsx
+++ b/tests/test-data/crosstab-mean-inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\dev\dataduck\tests\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E581888E-E184-416E-B7E0-9E9B205353AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7626911E-C7EC-4D52-9765-9D15F19E636D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="240" windowWidth="25665" windowHeight="20505" xr2:uid="{92061F1E-9ABC-447A-B522-1CC605CAA3B1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="38">
   <si>
     <t>HHINCOME_bucket</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>byrace</t>
+  </si>
+  <si>
+    <t>EXPECTED PERCENTS</t>
+  </si>
+  <si>
+    <t>EXPECTED COUNTS</t>
   </si>
 </sst>
 </file>
@@ -1029,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92983A33-11C6-4607-BD03-289812377F7B}">
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,136 +1530,71 @@
         <v>28</v>
       </c>
     </row>
+    <row r="16" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" t="s">
-        <v>24</v>
-      </c>
-      <c r="I18" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" t="s">
-        <v>25</v>
-      </c>
-      <c r="K18" t="s">
-        <v>26</v>
-      </c>
-      <c r="L18" t="s">
-        <v>27</v>
-      </c>
-      <c r="M18" t="s">
-        <v>28</v>
-      </c>
-      <c r="N18" t="s">
-        <v>30</v>
-      </c>
-      <c r="O18" t="s">
-        <v>31</v>
-      </c>
-      <c r="P18" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>33</v>
-      </c>
-      <c r="R18" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19">
         <v>2</v>
       </c>
-      <c r="D19">
-        <f>SUM(F2,F14)</f>
-        <v>65</v>
-      </c>
-      <c r="E19">
-        <f>SUM(G2,G14)</f>
-        <v>64</v>
-      </c>
-      <c r="F19">
-        <f>SUM(H2,H14)</f>
-        <v>71</v>
-      </c>
-      <c r="G19">
-        <f>SUM(I2,I14)</f>
-        <v>60</v>
-      </c>
-      <c r="H19">
-        <f>SUM(J2,J14)</f>
-        <v>64</v>
-      </c>
-      <c r="I19">
-        <f t="shared" ref="I19:J21" si="0">D19/SUM(D$19:D$21)*100</f>
-        <v>15.892420537897312</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="0"/>
-        <v>17.534246575342465</v>
-      </c>
-      <c r="K19">
-        <f t="shared" ref="K19:M21" si="1">F19/SUM(F$19:F$21)*100</f>
-        <v>17.401960784313726</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="1"/>
-        <v>14.084507042253522</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="1"/>
-        <v>16.202531645569621</v>
-      </c>
-      <c r="N19">
-        <f>(J19-$I19)^2</f>
-        <v>2.6955927372328521</v>
-      </c>
-      <c r="O19">
-        <f>(K19-$I19)^2</f>
-        <v>2.2787117555509275</v>
-      </c>
-      <c r="P19">
-        <f t="shared" ref="O19:Q23" si="2">(L19-$I19)^2</f>
-        <v>3.2685512077309489</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="2"/>
-        <v>9.6168899101746627E-2</v>
-      </c>
-      <c r="R19">
-        <f>SQRT((4/80)*SUM(N19:Q19))</f>
-        <v>0.64571760854170901</v>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" t="s">
+        <v>28</v>
+      </c>
+      <c r="N19" t="s">
+        <v>30</v>
+      </c>
+      <c r="O19" t="s">
+        <v>31</v>
+      </c>
+      <c r="P19" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>33</v>
+      </c>
+      <c r="R19" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -1661,70 +1602,70 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20">
-        <f>SUM(F4,F12)</f>
-        <v>116</v>
+        <f>SUM(F2,F14)</f>
+        <v>65</v>
       </c>
       <c r="E20">
-        <f>SUM(G4,G12)</f>
-        <v>84</v>
+        <f>SUM(G2,G14)</f>
+        <v>64</v>
       </c>
       <c r="F20">
-        <f>SUM(H4,H12)</f>
-        <v>110</v>
+        <f>SUM(H2,H14)</f>
+        <v>71</v>
       </c>
       <c r="G20">
-        <f>SUM(I4,I12)</f>
-        <v>111</v>
+        <f>SUM(I2,I14)</f>
+        <v>60</v>
       </c>
       <c r="H20">
-        <f>SUM(J4,J12)</f>
-        <v>109</v>
+        <f>SUM(J2,J14)</f>
+        <v>64</v>
       </c>
       <c r="I20">
-        <f t="shared" si="0"/>
-        <v>28.361858190709043</v>
+        <f t="shared" ref="I20:J22" si="0">D20/SUM(D$20:D$22)*100</f>
+        <v>15.892420537897312</v>
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>23.013698630136986</v>
+        <v>17.534246575342465</v>
       </c>
       <c r="K20">
-        <f t="shared" si="1"/>
-        <v>26.96078431372549</v>
+        <f t="shared" ref="K20:M22" si="1">F20/SUM(F$20:F$22)*100</f>
+        <v>17.401960784313726</v>
       </c>
       <c r="L20">
         <f t="shared" si="1"/>
-        <v>26.056338028169012</v>
+        <v>14.084507042253522</v>
       </c>
       <c r="M20">
         <f t="shared" si="1"/>
-        <v>27.594936708860761</v>
+        <v>16.202531645569621</v>
       </c>
       <c r="N20">
-        <f t="shared" ref="N20:N21" si="3">(J20-$I20)^2</f>
-        <v>28.602810685338298</v>
+        <f>(J20-$I20)^2</f>
+        <v>2.6955927372328521</v>
       </c>
       <c r="O20">
-        <f t="shared" si="2"/>
-        <v>1.9630080087657233</v>
+        <f>(K20-$I20)^2</f>
+        <v>2.2787117555509275</v>
       </c>
       <c r="P20">
-        <f t="shared" si="2"/>
-        <v>5.3154232198786096</v>
+        <f t="shared" ref="O20:Q24" si="2">(L20-$I20)^2</f>
+        <v>3.2685512077309489</v>
       </c>
       <c r="Q20">
         <f t="shared" si="2"/>
-        <v>0.58816855932036494</v>
+        <v>9.6168899101746627E-2</v>
       </c>
       <c r="R20">
-        <f t="shared" ref="R20:R23" si="4">SQRT((4/80)*SUM(N20:Q20))</f>
-        <v>1.3503594053677523</v>
+        <f>SQRT((4/80)*SUM(N20:Q20))</f>
+        <v>0.64571760854170901</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -1732,141 +1673,141 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <f>SUM(F4,F12)</f>
+        <v>116</v>
+      </c>
+      <c r="E21">
+        <f>SUM(G4,G12)</f>
+        <v>84</v>
+      </c>
+      <c r="F21">
+        <f>SUM(H4,H12)</f>
+        <v>110</v>
+      </c>
+      <c r="G21">
+        <f>SUM(I4,I12)</f>
+        <v>111</v>
+      </c>
+      <c r="H21">
+        <f>SUM(J4,J12)</f>
+        <v>109</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>28.361858190709043</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>23.013698630136986</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>26.96078431372549</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>26.056338028169012</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>27.594936708860761</v>
+      </c>
+      <c r="N21">
+        <f t="shared" ref="N21:N22" si="3">(J21-$I21)^2</f>
+        <v>28.602810685338298</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="2"/>
+        <v>1.9630080087657233</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="2"/>
+        <v>5.3154232198786096</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="2"/>
+        <v>0.58816855932036494</v>
+      </c>
+      <c r="R21">
+        <f t="shared" ref="R21:R24" si="4">SQRT((4/80)*SUM(N21:Q21))</f>
+        <v>1.3503594053677523</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
         <v>16</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>5</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <f>SUM(F5:F9)</f>
         <v>228</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <f>SUM(G5:G9)</f>
         <v>217</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <f>SUM(H5:H9)</f>
         <v>227</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <f>SUM(I5:I9)</f>
         <v>255</v>
       </c>
-      <c r="H21">
+      <c r="H22">
         <f>SUM(J5:J9)</f>
         <v>222</v>
       </c>
-      <c r="I21">
+      <c r="I22">
         <f t="shared" si="0"/>
         <v>55.745721271393641</v>
       </c>
-      <c r="J21">
+      <c r="J22">
         <f t="shared" si="0"/>
         <v>59.452054794520549</v>
       </c>
-      <c r="K21">
+      <c r="K22">
         <f t="shared" si="1"/>
         <v>55.637254901960787</v>
       </c>
-      <c r="L21">
+      <c r="L22">
         <f t="shared" si="1"/>
         <v>59.859154929577464</v>
       </c>
-      <c r="M21">
+      <c r="M22">
         <f t="shared" si="1"/>
         <v>56.202531645569621</v>
       </c>
-      <c r="N21">
+      <c r="N22">
         <f t="shared" si="3"/>
         <v>13.736908184654318</v>
       </c>
-      <c r="O21">
+      <c r="O22">
         <f t="shared" si="2"/>
         <v>1.1764953297944372E-2</v>
       </c>
-      <c r="P21">
+      <c r="P22">
         <f t="shared" si="2"/>
         <v>16.920336460279547</v>
       </c>
-      <c r="Q21">
+      <c r="Q22">
         <f t="shared" si="2"/>
         <v>0.20867571795479878</v>
       </c>
-      <c r="R21">
+      <c r="R22">
         <f t="shared" si="4"/>
         <v>1.2425313942952629</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22">
-        <f>SUM(F3,F10,F15)</f>
-        <v>106</v>
-      </c>
-      <c r="E22">
-        <f>SUM(G3,G10,G15)</f>
-        <v>129</v>
-      </c>
-      <c r="F22">
-        <f>SUM(H3,H10,H15)</f>
-        <v>106</v>
-      </c>
-      <c r="G22">
-        <f>SUM(I3,I10,I15)</f>
-        <v>103</v>
-      </c>
-      <c r="H22">
-        <f>SUM(J3,J10,J15)</f>
-        <v>102</v>
-      </c>
-      <c r="I22">
-        <f>D22/SUM(D$22:D$23)*100</f>
-        <v>51.707317073170735</v>
-      </c>
-      <c r="J22">
-        <f>E22/SUM(E$22:E$23)*100</f>
-        <v>57.589285714285708</v>
-      </c>
-      <c r="K22">
-        <f t="shared" ref="K22:M23" si="5">F22/SUM(F$22:F$23)*100</f>
-        <v>52.475247524752476</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="5"/>
-        <v>49.047619047619044</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="5"/>
-        <v>51</v>
-      </c>
-      <c r="N22">
-        <f>(J22-$I22)^2</f>
-        <v>34.597555095059924</v>
-      </c>
-      <c r="O22">
-        <f t="shared" si="2"/>
-        <v>0.58971717846653615</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="2"/>
-        <v>7.0739935871235637</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" si="2"/>
-        <v>0.50029744199881487</v>
-      </c>
-      <c r="R22">
-        <f t="shared" si="4"/>
-        <v>1.46221686665571</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -1874,54 +1815,54 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D23">
-        <f>SUM(F11,F13)</f>
-        <v>99</v>
+        <f>SUM(F3,F10,F15)</f>
+        <v>106</v>
       </c>
       <c r="E23">
-        <f>SUM(G11,G13)</f>
-        <v>95</v>
+        <f>SUM(G3,G10,G15)</f>
+        <v>129</v>
       </c>
       <c r="F23">
-        <f>SUM(H11,H13)</f>
-        <v>96</v>
+        <f>SUM(H3,H10,H15)</f>
+        <v>106</v>
       </c>
       <c r="G23">
-        <f>SUM(I11,I13)</f>
-        <v>107</v>
+        <f>SUM(I3,I10,I15)</f>
+        <v>103</v>
       </c>
       <c r="H23">
-        <f>SUM(J11,J13)</f>
-        <v>98</v>
+        <f>SUM(J3,J10,J15)</f>
+        <v>102</v>
       </c>
       <c r="I23">
-        <f>D23/SUM(D$22:D$23)*100</f>
-        <v>48.292682926829265</v>
+        <f>D23/SUM(D$23:D$24)*100</f>
+        <v>51.707317073170735</v>
       </c>
       <c r="J23">
-        <f>E23/SUM(E$22:E$23)*100</f>
-        <v>42.410714285714285</v>
+        <f>E23/SUM(E$23:E$24)*100</f>
+        <v>57.589285714285708</v>
       </c>
       <c r="K23">
-        <f t="shared" si="5"/>
-        <v>47.524752475247524</v>
+        <f t="shared" ref="K23:M24" si="5">F23/SUM(F$23:F$24)*100</f>
+        <v>52.475247524752476</v>
       </c>
       <c r="L23">
         <f t="shared" si="5"/>
-        <v>50.952380952380949</v>
+        <v>49.047619047619044</v>
       </c>
       <c r="M23">
         <f t="shared" si="5"/>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N23">
         <f>(J23-$I23)^2</f>
-        <v>34.597555095060009</v>
+        <v>34.597555095059924</v>
       </c>
       <c r="O23">
         <f t="shared" si="2"/>
@@ -1929,7 +1870,7 @@
       </c>
       <c r="P23">
         <f t="shared" si="2"/>
-        <v>7.0739935871235264</v>
+        <v>7.0739935871235637</v>
       </c>
       <c r="Q23">
         <f t="shared" si="2"/>
@@ -1937,134 +1878,139 @@
       </c>
       <c r="R23">
         <f t="shared" si="4"/>
+        <v>1.46221686665571</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <f>SUM(F11,F13)</f>
+        <v>99</v>
+      </c>
+      <c r="E24">
+        <f>SUM(G11,G13)</f>
+        <v>95</v>
+      </c>
+      <c r="F24">
+        <f>SUM(H11,H13)</f>
+        <v>96</v>
+      </c>
+      <c r="G24">
+        <f>SUM(I11,I13)</f>
+        <v>107</v>
+      </c>
+      <c r="H24">
+        <f>SUM(J11,J13)</f>
+        <v>98</v>
+      </c>
+      <c r="I24">
+        <f>D24/SUM(D$23:D$24)*100</f>
+        <v>48.292682926829265</v>
+      </c>
+      <c r="J24">
+        <f>E24/SUM(E$23:E$24)*100</f>
+        <v>42.410714285714285</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="5"/>
+        <v>47.524752475247524</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="5"/>
+        <v>50.952380952380949</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="5"/>
+        <v>49</v>
+      </c>
+      <c r="N24">
+        <f>(J24-$I24)^2</f>
+        <v>34.597555095060009</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="2"/>
+        <v>0.58971717846653615</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="2"/>
+        <v>7.0739935871235264</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="2"/>
+        <v>0.50029744199881487</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="4"/>
         <v>1.4622168666557107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" t="s">
-        <v>23</v>
-      </c>
-      <c r="H26" t="s">
-        <v>24</v>
-      </c>
-      <c r="I26" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" t="s">
-        <v>25</v>
-      </c>
-      <c r="K26" t="s">
-        <v>26</v>
-      </c>
-      <c r="L26" t="s">
-        <v>27</v>
-      </c>
-      <c r="M26" t="s">
-        <v>28</v>
-      </c>
-      <c r="N26" t="s">
-        <v>30</v>
-      </c>
-      <c r="O26" t="s">
-        <v>31</v>
-      </c>
-      <c r="P26" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>33</v>
-      </c>
-      <c r="R26" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27">
-        <v>65</v>
-      </c>
-      <c r="E27">
-        <v>64</v>
-      </c>
-      <c r="F27">
-        <v>71</v>
-      </c>
-      <c r="G27">
-        <v>60</v>
-      </c>
-      <c r="H27">
-        <v>64</v>
-      </c>
-      <c r="I27">
-        <f>D27/SUM(D$27)*100</f>
-        <v>100</v>
-      </c>
-      <c r="J27">
-        <f t="shared" ref="J27:M27" si="6">E27/SUM(E$27)*100</f>
-        <v>100</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="6"/>
-        <v>100</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="6"/>
-        <v>100</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="6"/>
-        <v>100</v>
-      </c>
-      <c r="N27">
-        <f>(J27-$I27)^2</f>
-        <v>0</v>
-      </c>
-      <c r="O27">
-        <f>(K27-$I27)^2</f>
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <f t="shared" ref="P27:P31" si="7">(L27-$I27)^2</f>
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" ref="Q27:Q31" si="8">(M27-$I27)^2</f>
-        <v>0</v>
-      </c>
-      <c r="R27">
-        <f>SQRT((4/80)*SUM(N27:Q27))</f>
-        <v>0</v>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J27" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" t="s">
+        <v>27</v>
+      </c>
+      <c r="M27" t="s">
+        <v>28</v>
+      </c>
+      <c r="N27" t="s">
+        <v>30</v>
+      </c>
+      <c r="O27" t="s">
+        <v>31</v>
+      </c>
+      <c r="P27" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>33</v>
+      </c>
+      <c r="R27" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -2072,65 +2018,65 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="E28">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="F28">
-        <v>110</v>
+        <v>71</v>
       </c>
       <c r="G28">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="H28">
-        <v>109</v>
+        <v>64</v>
       </c>
       <c r="I28">
-        <f>D28/SUM(D$28,D$30)*100</f>
-        <v>52.252252252252248</v>
+        <f>D28/SUM(D$28)*100</f>
+        <v>100</v>
       </c>
       <c r="J28">
-        <f t="shared" ref="J28:M28" si="9">E28/SUM(E$28,E$30)*100</f>
-        <v>39.436619718309856</v>
+        <f t="shared" ref="J28:M28" si="6">E28/SUM(E$28)*100</f>
+        <v>100</v>
       </c>
       <c r="K28">
-        <f t="shared" si="9"/>
-        <v>50.925925925925931</v>
+        <f t="shared" si="6"/>
+        <v>100</v>
       </c>
       <c r="L28">
-        <f t="shared" si="9"/>
-        <v>51.86915887850467</v>
+        <f t="shared" si="6"/>
+        <v>100</v>
       </c>
       <c r="M28">
-        <f t="shared" si="9"/>
-        <v>51.658767772511851</v>
+        <f t="shared" si="6"/>
+        <v>100</v>
       </c>
       <c r="N28">
-        <f t="shared" ref="N28:N29" si="10">(J28-$I28)^2</f>
-        <v>164.24043724504267</v>
+        <f>(J28-$I28)^2</f>
+        <v>0</v>
       </c>
       <c r="O28">
-        <f t="shared" ref="O28:O31" si="11">(K28-$I28)^2</f>
-        <v>1.7591415239062638</v>
+        <f>(K28-$I28)^2</f>
+        <v>0</v>
       </c>
       <c r="P28">
-        <f t="shared" si="7"/>
-        <v>0.14676053300930106</v>
+        <f t="shared" ref="P28:P32" si="7">(L28-$I28)^2</f>
+        <v>0</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="8"/>
-        <v>0.35222382769272953</v>
+        <f t="shared" ref="Q28:Q32" si="8">(M28-$I28)^2</f>
+        <v>0</v>
       </c>
       <c r="R28">
-        <f t="shared" ref="R28:R31" si="12">SQRT((4/80)*SUM(N28:Q28))</f>
-        <v>2.8852951593350982</v>
+        <f>SQRT((4/80)*SUM(N28:Q28))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -2138,131 +2084,131 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>116</v>
+      </c>
+      <c r="E29">
+        <v>84</v>
+      </c>
+      <c r="F29">
+        <v>110</v>
+      </c>
+      <c r="G29">
+        <v>111</v>
+      </c>
+      <c r="H29">
+        <v>109</v>
+      </c>
+      <c r="I29">
+        <f>D29/SUM(D$29,D$31)*100</f>
+        <v>52.252252252252248</v>
+      </c>
+      <c r="J29">
+        <f t="shared" ref="J29:M29" si="9">E29/SUM(E$29,E$31)*100</f>
+        <v>39.436619718309856</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="9"/>
+        <v>50.925925925925931</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="9"/>
+        <v>51.86915887850467</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="9"/>
+        <v>51.658767772511851</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ref="N29:N30" si="10">(J29-$I29)^2</f>
+        <v>164.24043724504267</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ref="O29:O32" si="11">(K29-$I29)^2</f>
+        <v>1.7591415239062638</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="7"/>
+        <v>0.14676053300930106</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="8"/>
+        <v>0.35222382769272953</v>
+      </c>
+      <c r="R29">
+        <f t="shared" ref="R29:R32" si="12">SQRT((4/80)*SUM(N29:Q29))</f>
+        <v>2.8852951593350982</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
         <v>16</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <v>5</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>228</v>
       </c>
-      <c r="E29">
+      <c r="E30">
         <v>217</v>
       </c>
-      <c r="F29">
+      <c r="F30">
         <v>227</v>
       </c>
-      <c r="G29">
+      <c r="G30">
         <v>255</v>
       </c>
-      <c r="H29">
+      <c r="H30">
         <v>222</v>
       </c>
-      <c r="I29">
-        <f>D$29/SUM(D$29)*100</f>
+      <c r="I30">
+        <f>D$30/SUM(D$30)*100</f>
         <v>100</v>
       </c>
-      <c r="J29">
-        <f t="shared" ref="J29:M29" si="13">E$29/SUM(E$29)*100</f>
+      <c r="J30">
+        <f t="shared" ref="J30:M30" si="13">E$30/SUM(E$30)*100</f>
         <v>100</v>
       </c>
-      <c r="K29">
+      <c r="K30">
         <f t="shared" si="13"/>
         <v>100</v>
       </c>
-      <c r="L29">
+      <c r="L30">
         <f t="shared" si="13"/>
         <v>100</v>
       </c>
-      <c r="M29">
+      <c r="M30">
         <f t="shared" si="13"/>
         <v>100</v>
       </c>
-      <c r="N29">
+      <c r="N30">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O29">
+      <c r="O30">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P29">
+      <c r="P30">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q29">
+      <c r="Q30">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="R29">
+      <c r="R30">
         <f t="shared" si="12"/>
         <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30">
-        <v>3</v>
-      </c>
-      <c r="D30">
-        <v>106</v>
-      </c>
-      <c r="E30">
-        <v>129</v>
-      </c>
-      <c r="F30">
-        <v>106</v>
-      </c>
-      <c r="G30">
-        <v>103</v>
-      </c>
-      <c r="H30">
-        <v>102</v>
-      </c>
-      <c r="I30">
-        <f>D30/SUM(D$28,D$30)*100</f>
-        <v>47.747747747747752</v>
-      </c>
-      <c r="J30">
-        <f t="shared" ref="J30" si="14">E30/SUM(E$28,E$30)*100</f>
-        <v>60.563380281690137</v>
-      </c>
-      <c r="K30">
-        <f t="shared" ref="K30" si="15">F30/SUM(F$28,F$30)*100</f>
-        <v>49.074074074074076</v>
-      </c>
-      <c r="L30">
-        <f t="shared" ref="L30" si="16">G30/SUM(G$28,G$30)*100</f>
-        <v>48.13084112149533</v>
-      </c>
-      <c r="M30">
-        <f t="shared" ref="M30" si="17">H30/SUM(H$28,H$30)*100</f>
-        <v>48.341232227488149</v>
-      </c>
-      <c r="N30">
-        <f>(J30-$I30)^2</f>
-        <v>164.2404372450425</v>
-      </c>
-      <c r="O30">
-        <f t="shared" si="11"/>
-        <v>1.7591415239062826</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="7"/>
-        <v>0.14676053300930106</v>
-      </c>
-      <c r="Q30">
-        <f t="shared" si="8"/>
-        <v>0.35222382769272953</v>
-      </c>
-      <c r="R30">
-        <f t="shared" si="12"/>
-        <v>2.8852951593350968</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -2270,65 +2216,407 @@
         <v>13</v>
       </c>
       <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>106</v>
+      </c>
+      <c r="E31">
+        <v>129</v>
+      </c>
+      <c r="F31">
+        <v>106</v>
+      </c>
+      <c r="G31">
+        <v>103</v>
+      </c>
+      <c r="H31">
+        <v>102</v>
+      </c>
+      <c r="I31">
+        <f>D31/SUM(D$29,D$31)*100</f>
+        <v>47.747747747747752</v>
+      </c>
+      <c r="J31">
+        <f t="shared" ref="J31" si="14">E31/SUM(E$29,E$31)*100</f>
+        <v>60.563380281690137</v>
+      </c>
+      <c r="K31">
+        <f t="shared" ref="K31" si="15">F31/SUM(F$29,F$31)*100</f>
+        <v>49.074074074074076</v>
+      </c>
+      <c r="L31">
+        <f t="shared" ref="L31" si="16">G31/SUM(G$29,G$31)*100</f>
+        <v>48.13084112149533</v>
+      </c>
+      <c r="M31">
+        <f t="shared" ref="M31" si="17">H31/SUM(H$29,H$31)*100</f>
+        <v>48.341232227488149</v>
+      </c>
+      <c r="N31">
+        <f>(J31-$I31)^2</f>
+        <v>164.2404372450425</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="11"/>
+        <v>1.7591415239062826</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="7"/>
+        <v>0.14676053300930106</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="8"/>
+        <v>0.35222382769272953</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="12"/>
+        <v>2.8852951593350968</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
         <v>17</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>2</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>99</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <v>95</v>
       </c>
-      <c r="F31">
+      <c r="F32">
         <v>96</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <v>107</v>
       </c>
-      <c r="H31">
+      <c r="H32">
         <v>98</v>
       </c>
-      <c r="I31">
-        <f>D31/SUM(D$31)*100</f>
+      <c r="I32">
+        <f>D32/SUM(D$32)*100</f>
         <v>100</v>
       </c>
-      <c r="J31">
-        <f t="shared" ref="J31:M31" si="18">E31/SUM(E$31)*100</f>
+      <c r="J32">
+        <f t="shared" ref="J32:M32" si="18">E32/SUM(E$32)*100</f>
         <v>100</v>
       </c>
-      <c r="K31">
+      <c r="K32">
         <f t="shared" si="18"/>
         <v>100</v>
       </c>
-      <c r="L31">
+      <c r="L32">
         <f t="shared" si="18"/>
         <v>100</v>
       </c>
-      <c r="M31">
+      <c r="M32">
         <f t="shared" si="18"/>
         <v>100</v>
       </c>
-      <c r="N31">
-        <f>(J31-$I31)^2</f>
+      <c r="N32">
+        <f>(J32-$I32)^2</f>
         <v>0</v>
       </c>
-      <c r="O31">
+      <c r="O32">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P31">
+      <c r="P32">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q31">
+      <c r="Q32">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="R31">
+      <c r="R32">
         <f t="shared" si="12"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" t="s">
+        <v>24</v>
+      </c>
+      <c r="I35" t="s">
+        <v>30</v>
+      </c>
+      <c r="J35" t="s">
+        <v>31</v>
+      </c>
+      <c r="K35" t="s">
+        <v>32</v>
+      </c>
+      <c r="L35" t="s">
+        <v>33</v>
+      </c>
+      <c r="M35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>65</v>
+      </c>
+      <c r="E36">
+        <v>64</v>
+      </c>
+      <c r="F36">
+        <v>71</v>
+      </c>
+      <c r="G36">
+        <v>60</v>
+      </c>
+      <c r="H36">
+        <v>64</v>
+      </c>
+      <c r="I36">
+        <f>(E36-$D36)^2</f>
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <f>(F36-$D36)^2</f>
+        <v>36</v>
+      </c>
+      <c r="K36">
+        <f t="shared" ref="K36:L40" si="19">(G36-$D36)^2</f>
+        <v>25</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <f>SQRT((4/80)*SUM(I36:L36))</f>
+        <v>1.7748239349298849</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>116</v>
+      </c>
+      <c r="E37">
+        <v>84</v>
+      </c>
+      <c r="F37">
+        <v>110</v>
+      </c>
+      <c r="G37">
+        <v>111</v>
+      </c>
+      <c r="H37">
+        <v>109</v>
+      </c>
+      <c r="I37">
+        <f>(E37-$D37)^2</f>
+        <v>1024</v>
+      </c>
+      <c r="J37">
+        <f>(F37-$D37)^2</f>
+        <v>36</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="19"/>
+        <v>25</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="19"/>
+        <v>49</v>
+      </c>
+      <c r="M37">
+        <f t="shared" ref="M37:M40" si="20">SQRT((4/80)*SUM(I37:L37))</f>
+        <v>7.5299402388066801</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>228</v>
+      </c>
+      <c r="E38">
+        <v>217</v>
+      </c>
+      <c r="F38">
+        <v>227</v>
+      </c>
+      <c r="G38">
+        <v>255</v>
+      </c>
+      <c r="H38">
+        <v>222</v>
+      </c>
+      <c r="I38">
+        <f t="shared" ref="I37:J40" si="21">(E38-$D38)^2</f>
+        <v>121</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="19"/>
+        <v>729</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="19"/>
+        <v>36</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="20"/>
+        <v>6.6595795663089721</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>106</v>
+      </c>
+      <c r="E39">
+        <v>129</v>
+      </c>
+      <c r="F39">
+        <v>106</v>
+      </c>
+      <c r="G39">
+        <v>103</v>
+      </c>
+      <c r="H39">
+        <v>102</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="21"/>
+        <v>529</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="19"/>
+        <v>9</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="19"/>
+        <v>16</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="20"/>
+        <v>5.2630789467763073</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>99</v>
+      </c>
+      <c r="E40">
+        <v>95</v>
+      </c>
+      <c r="F40">
+        <v>96</v>
+      </c>
+      <c r="G40">
+        <v>107</v>
+      </c>
+      <c r="H40">
+        <v>98</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="21"/>
+        <v>16</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="19"/>
+        <v>64</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="20"/>
+        <v>2.1213203435596424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(unit test): add expected mean standard errors to (failing) unit test
This test is for the `crosstab_mean()` function
</commit_message>
<xml_diff>
--- a/tests/test-data/crosstab-mean-inputs.xlsx
+++ b/tests/test-data/crosstab-mean-inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\dev\dataduck\tests\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7626911E-C7EC-4D52-9765-9D15F19E636D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F0B14A-EAD4-4D5C-9D96-E6BEAFBCAEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="240" windowWidth="25665" windowHeight="20505" xr2:uid="{92061F1E-9ABC-447A-B522-1CC605CAA3B1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="44">
   <si>
     <t>HHINCOME_bucket</t>
   </si>
@@ -147,13 +147,31 @@
   </si>
   <si>
     <t>EXPECTED COUNTS</t>
+  </si>
+  <si>
+    <t>EXPECTED MEANS</t>
+  </si>
+  <si>
+    <t>weighted_mean</t>
+  </si>
+  <si>
+    <t>wm1</t>
+  </si>
+  <si>
+    <t>wm2</t>
+  </si>
+  <si>
+    <t>wm3</t>
+  </si>
+  <si>
+    <t>wm4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +302,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1035,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92983A33-11C6-4607-BD03-289812377F7B}">
-  <dimension ref="A1:R40"/>
+  <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S47" sqref="S47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,6 +1070,11 @@
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2343,12 +2372,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -2389,7 +2418,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2435,7 +2464,7 @@
         <v>1.7748239349298849</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2481,7 +2510,7 @@
         <v>7.5299402388066801</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2507,7 +2536,7 @@
         <v>222</v>
       </c>
       <c r="I38">
-        <f t="shared" ref="I37:J40" si="21">(E38-$D38)^2</f>
+        <f t="shared" ref="I38:J40" si="21">(E38-$D38)^2</f>
         <v>121</v>
       </c>
       <c r="J38">
@@ -2527,7 +2556,7 @@
         <v>6.6595795663089721</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -2573,7 +2602,7 @@
         <v>5.2630789467763073</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -2619,7 +2648,417 @@
         <v>2.1213203435596424</v>
       </c>
     </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" t="s">
+        <v>23</v>
+      </c>
+      <c r="H43" t="s">
+        <v>24</v>
+      </c>
+      <c r="I43" t="s">
+        <v>19</v>
+      </c>
+      <c r="J43" t="s">
+        <v>39</v>
+      </c>
+      <c r="K43" t="s">
+        <v>40</v>
+      </c>
+      <c r="L43" t="s">
+        <v>41</v>
+      </c>
+      <c r="M43" t="s">
+        <v>42</v>
+      </c>
+      <c r="N43" t="s">
+        <v>43</v>
+      </c>
+      <c r="O43" t="s">
+        <v>30</v>
+      </c>
+      <c r="P43" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>32</v>
+      </c>
+      <c r="R43" t="s">
+        <v>33</v>
+      </c>
+      <c r="S43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44">
+        <v>65</v>
+      </c>
+      <c r="E44">
+        <v>64</v>
+      </c>
+      <c r="F44">
+        <v>71</v>
+      </c>
+      <c r="G44">
+        <v>60</v>
+      </c>
+      <c r="H44">
+        <v>64</v>
+      </c>
+      <c r="I44">
+        <v>2</v>
+      </c>
+      <c r="J44">
+        <f>(F2*$E2+F14*$E14)/D44</f>
+        <v>2.6</v>
+      </c>
+      <c r="K44">
+        <f>(G2*$E2+G14*$E14)/E44</f>
+        <v>2.625</v>
+      </c>
+      <c r="L44">
+        <f t="shared" ref="K44:N44" si="22">(H2*$E2+H14*$E14)/F44</f>
+        <v>2.6338028169014085</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="22"/>
+        <v>2.5833333333333335</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="22"/>
+        <v>2.515625</v>
+      </c>
+      <c r="O44">
+        <f>(K44-$J44)^2</f>
+        <v>6.2499999999999557E-4</v>
+      </c>
+      <c r="P44">
+        <f>(L44-$J44)^2</f>
+        <v>1.1426304304701417E-3</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" ref="P44:R48" si="23">(M44-$J44)^2</f>
+        <v>2.7777777777777583E-4</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="23"/>
+        <v>7.1191406250000148E-3</v>
+      </c>
+      <c r="S44">
+        <f>SQRT((4/80)*SUM(O44:R44))</f>
+        <v>2.1406247724960963E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45">
+        <v>116</v>
+      </c>
+      <c r="E45">
+        <v>84</v>
+      </c>
+      <c r="F45">
+        <v>110</v>
+      </c>
+      <c r="G45">
+        <v>111</v>
+      </c>
+      <c r="H45">
+        <v>109</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="J45">
+        <f>(F4*$E4+F12*$E12)/D45</f>
+        <v>2.6120689655172415</v>
+      </c>
+      <c r="K45">
+        <f>(G4*$E4+G12*$E12)/E45</f>
+        <v>2.7023809523809526</v>
+      </c>
+      <c r="L45">
+        <f t="shared" ref="K45:N45" si="24">(H4*$E4+H12*$E12)/F45</f>
+        <v>2.6</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="24"/>
+        <v>2.6306306306306309</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="24"/>
+        <v>2.6146788990825689</v>
+      </c>
+      <c r="O45">
+        <f>(K45-$J45)^2</f>
+        <v>8.1562549712711086E-3</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="23"/>
+        <v>1.4565992865636339E-4</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="23"/>
+        <v>3.4453541178161351E-4</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="23"/>
+        <v>6.8117532154223289E-6</v>
+      </c>
+      <c r="S45">
+        <f t="shared" ref="S45:S48" si="25">SQRT((4/80)*SUM(O45:R45))</f>
+        <v>2.0800555359081773E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46">
+        <v>106</v>
+      </c>
+      <c r="E46">
+        <v>129</v>
+      </c>
+      <c r="F46">
+        <v>106</v>
+      </c>
+      <c r="G46">
+        <v>103</v>
+      </c>
+      <c r="H46">
+        <v>102</v>
+      </c>
+      <c r="I46">
+        <v>3</v>
+      </c>
+      <c r="J46">
+        <f>((F3*$E3)+($E10*F10)+(F15*$E15))/D46</f>
+        <v>1.8773584905660377</v>
+      </c>
+      <c r="K46">
+        <f t="shared" ref="K46:N46" si="26">((G3*$E3)+($E10*G10)+(G15*$E15))/E46</f>
+        <v>1.9534883720930232</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="26"/>
+        <v>1.9056603773584906</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="26"/>
+        <v>1.8737864077669903</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="26"/>
+        <v>1.9019607843137254</v>
+      </c>
+      <c r="O46">
+        <f>(K46-$J46)^2</f>
+        <v>5.7957588613128516E-3</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="23"/>
+        <v>8.0099679601282185E-4</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="23"/>
+        <v>1.2759775523249627E-5</v>
+      </c>
+      <c r="R46">
+        <f>(N46-$J46)^2</f>
+        <v>6.0527285764751541E-4</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="25"/>
+        <v>1.8993141249535894E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47">
+        <v>99</v>
+      </c>
+      <c r="E47">
+        <v>95</v>
+      </c>
+      <c r="F47">
+        <v>96</v>
+      </c>
+      <c r="G47">
+        <v>107</v>
+      </c>
+      <c r="H47">
+        <v>98</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+      <c r="J47">
+        <f>(F11*$E11+F13*$E13)/D47</f>
+        <v>1.6565656565656566</v>
+      </c>
+      <c r="K47">
+        <f t="shared" ref="K47:N47" si="27">(G11*$E11+G13*$E13)/E47</f>
+        <v>1.6947368421052631</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="27"/>
+        <v>1.625</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="27"/>
+        <v>1.6542056074766356</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="27"/>
+        <v>1.6938775510204083</v>
+      </c>
+      <c r="O47">
+        <f>(K47-$J47)^2</f>
+        <v>1.457039405499066E-3</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="23"/>
+        <v>9.9639067442097804E-4</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="23"/>
+        <v>5.5698317025887951E-6</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="23"/>
+        <v>1.3921774678025301E-3</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="25"/>
+        <v>1.3876558253805522E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48">
+        <v>228</v>
+      </c>
+      <c r="E48">
+        <v>217</v>
+      </c>
+      <c r="F48">
+        <v>227</v>
+      </c>
+      <c r="G48">
+        <v>255</v>
+      </c>
+      <c r="H48">
+        <v>222</v>
+      </c>
+      <c r="I48">
+        <v>5</v>
+      </c>
+      <c r="J48">
+        <f>SUMPRODUCT(F5:F9,$E5:$E9)/D48</f>
+        <v>5</v>
+      </c>
+      <c r="K48">
+        <f t="shared" ref="K48:N48" si="28">SUMPRODUCT(G5:G9,$E5:$E9)/E48</f>
+        <v>5</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="28"/>
+        <v>5</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="28"/>
+        <v>5</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="28"/>
+        <v>5</v>
+      </c>
+      <c r="O48">
+        <f>(K48-$J48)^2</f>
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>